<commit_message>
Added sorting and pattern
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Placement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CFE844-C610-4348-B6E1-2FF372A01EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB1268D-9289-43D1-8C75-0C9C89FF560E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2702" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="467">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1545,7 +1545,57 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1857,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="104" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2454,7 +2504,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="21">
@@ -2465,7 +2515,7 @@
         <v>58</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="21">
@@ -2476,7 +2526,7 @@
         <v>59</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="21">
@@ -2487,7 +2537,7 @@
         <v>60</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="21">
@@ -2498,7 +2548,7 @@
         <v>61</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="21">
@@ -6924,6 +6974,29 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C6:C481">
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>C$6</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>$C1048107</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>$C1048107 = "Yes"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="&lt;-&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;-&gt;",C6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="&lt;-&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;-&gt;",C6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",C6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>
     <hyperlink ref="B7" r:id="rId2" xr:uid="{2D6F1134-3C08-7445-B19A-9B94A18B55C7}"/>

</xml_diff>